<commit_message>
Implemented FragilityCurve and Hazard modules
</commit_message>
<xml_diff>
--- a/jupyter_notebooks/file/input/basic_example/network.xlsx
+++ b/jupyter_notebooks/file/input/basic_example/network.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FBK106\Documents\Repositories\ResiliencyTool\jupyter_notebooks\file\input\example_1.2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\ResiliencyTool\jupyter_notebooks\file\input\basic_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D13C7A-87CC-4CB2-BC15-2968A9635F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904ED986-C428-4E49-9DA6-32237F7B741F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{9ECEC293-7360-4DDE-9C10-8A2C51BA16DF}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="165">
   <si>
     <t>name</t>
   </si>
@@ -533,6 +533,15 @@
   </si>
   <si>
     <t>slack</t>
+  </si>
+  <si>
+    <t>tower_type1</t>
+  </si>
+  <si>
+    <t>tower_type2</t>
+  </si>
+  <si>
+    <t>tower_type3</t>
   </si>
 </sst>
 </file>
@@ -4627,7 +4636,7 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4697,12 +4706,10 @@
         <v>220</v>
       </c>
       <c r="D2">
-        <f>D3+0.5</f>
-        <v>81.400000000000006</v>
+        <v>8.58</v>
       </c>
       <c r="E2">
-        <f>E3</f>
-        <v>9.5</v>
+        <v>52.71</v>
       </c>
       <c r="G2">
         <v>1.1000000000000001</v>
@@ -4728,10 +4735,10 @@
         <v>110</v>
       </c>
       <c r="D3">
-        <v>80.900000000000006</v>
+        <v>8.66</v>
       </c>
       <c r="E3">
-        <v>9.5</v>
+        <v>52.28</v>
       </c>
       <c r="G3">
         <v>1.1000000000000001</v>
@@ -4751,12 +4758,10 @@
         <v>110</v>
       </c>
       <c r="D4">
-        <f>D3-P2</f>
-        <v>79.900000000000006</v>
+        <v>8.76</v>
       </c>
       <c r="E4">
-        <f>E3</f>
-        <v>9.5</v>
+        <v>52.65</v>
       </c>
       <c r="G4">
         <v>1.1000000000000001</v>
@@ -4776,12 +4781,10 @@
         <v>110</v>
       </c>
       <c r="D5">
-        <f>D4</f>
-        <v>79.900000000000006</v>
+        <v>9.68</v>
       </c>
       <c r="E5">
-        <f>E4+O2</f>
-        <v>10.5</v>
+        <v>51.59</v>
       </c>
       <c r="G5">
         <v>1.1000000000000001</v>
@@ -4801,12 +4804,10 @@
         <v>110</v>
       </c>
       <c r="D6">
-        <f>D5</f>
-        <v>79.900000000000006</v>
+        <v>10.62</v>
       </c>
       <c r="E6">
-        <f>E5+O2</f>
-        <v>11.5</v>
+        <v>51.57</v>
       </c>
       <c r="G6">
         <v>1.1000000000000001</v>
@@ -4826,12 +4827,10 @@
         <v>110</v>
       </c>
       <c r="D7">
-        <f>D6</f>
-        <v>79.900000000000006</v>
+        <v>11.43</v>
       </c>
       <c r="E7">
-        <f>E6+O2</f>
-        <v>12.5</v>
+        <v>51.52</v>
       </c>
       <c r="G7">
         <v>1.1000000000000001</v>
@@ -4851,12 +4850,10 @@
         <v>110</v>
       </c>
       <c r="D8">
-        <f>D6-P2</f>
-        <v>78.900000000000006</v>
+        <v>10.67</v>
       </c>
       <c r="E8">
-        <f>E6</f>
-        <v>11.5</v>
+        <v>50.9</v>
       </c>
       <c r="G8">
         <v>1.1000000000000001</v>
@@ -4876,12 +4873,10 @@
         <v>110</v>
       </c>
       <c r="D9">
-        <f>D8-P2</f>
-        <v>77.900000000000006</v>
+        <v>10.67</v>
       </c>
       <c r="E9">
-        <f>E8</f>
-        <v>11.5</v>
+        <v>50.45</v>
       </c>
       <c r="G9">
         <v>1.1000000000000001</v>
@@ -4901,12 +4896,10 @@
         <v>110</v>
       </c>
       <c r="D10">
-        <f>D9-P2</f>
-        <v>76.900000000000006</v>
+        <v>10.88</v>
       </c>
       <c r="E10">
-        <f>E9</f>
-        <v>11.5</v>
+        <v>49.94</v>
       </c>
       <c r="G10">
         <v>1.1000000000000001</v>
@@ -4926,12 +4919,10 @@
         <v>110</v>
       </c>
       <c r="D11">
-        <f>D4-P2</f>
-        <v>78.900000000000006</v>
+        <v>8.32</v>
       </c>
       <c r="E11">
-        <f>E4</f>
-        <v>9.5</v>
+        <v>51.26</v>
       </c>
       <c r="G11">
         <v>1.1000000000000001</v>
@@ -4951,12 +4942,10 @@
         <v>110</v>
       </c>
       <c r="D12">
-        <f>D11</f>
-        <v>78.900000000000006</v>
+        <v>7.51</v>
       </c>
       <c r="E12">
-        <f>E11-O2</f>
-        <v>8.5</v>
+        <v>51.21</v>
       </c>
       <c r="G12">
         <v>1.1000000000000001</v>
@@ -4976,12 +4965,10 @@
         <v>110</v>
       </c>
       <c r="D13">
-        <f>D11-P2</f>
-        <v>77.900000000000006</v>
+        <v>8.59</v>
       </c>
       <c r="E13">
-        <f>E11</f>
-        <v>9.5</v>
+        <v>50.66</v>
       </c>
       <c r="G13">
         <v>1.1000000000000001</v>
@@ -5001,12 +4988,10 @@
         <v>110</v>
       </c>
       <c r="D14">
-        <f>D13-P2</f>
-        <v>76.900000000000006</v>
+        <v>8.7899999999999991</v>
       </c>
       <c r="E14">
-        <f>E13</f>
-        <v>9.5</v>
+        <v>49.93</v>
       </c>
       <c r="G14">
         <v>1.1000000000000001</v>
@@ -5026,12 +5011,10 @@
         <v>110</v>
       </c>
       <c r="D15">
-        <f>D14</f>
-        <v>76.900000000000006</v>
+        <v>7.88</v>
       </c>
       <c r="E15">
-        <f>E14-O2</f>
-        <v>8.5</v>
+        <v>49.91</v>
       </c>
       <c r="G15">
         <v>1.1000000000000001</v>
@@ -5051,12 +5034,10 @@
         <v>110</v>
       </c>
       <c r="D16">
-        <f>D14-P2</f>
-        <v>75.900000000000006</v>
+        <v>8.7799999999999994</v>
       </c>
       <c r="E16">
-        <f>E14</f>
-        <v>9.5</v>
+        <v>49.37</v>
       </c>
       <c r="G16">
         <v>1.1000000000000001</v>
@@ -5076,12 +5057,10 @@
         <v>110</v>
       </c>
       <c r="D17">
-        <f>D16</f>
-        <v>75.900000000000006</v>
+        <v>7.6</v>
       </c>
       <c r="E17">
-        <f>E16-O2</f>
-        <v>8.5</v>
+        <v>49.33</v>
       </c>
       <c r="G17">
         <v>1.1000000000000001</v>
@@ -5101,12 +5080,10 @@
         <v>110</v>
       </c>
       <c r="D18">
-        <f>D16-P2</f>
-        <v>74.900000000000006</v>
+        <v>8.92</v>
       </c>
       <c r="E18">
-        <f>E16</f>
-        <v>9.5</v>
+        <v>48.75</v>
       </c>
       <c r="G18">
         <v>1.1000000000000001</v>
@@ -5126,12 +5103,10 @@
         <v>110</v>
       </c>
       <c r="D19">
-        <f>D9</f>
-        <v>77.900000000000006</v>
+        <v>11.64</v>
       </c>
       <c r="E19">
-        <f>E9+O2</f>
-        <v>12.5</v>
+        <v>50.39</v>
       </c>
       <c r="G19">
         <v>1.1000000000000001</v>
@@ -5155,7 +5130,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5415,10 +5390,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB5B7B5-BF13-4654-A134-6B30DC3D029F}">
-  <dimension ref="A1:X8"/>
+  <dimension ref="A1:Y8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5444,11 +5419,12 @@
     <col min="19" max="19" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5516,13 +5492,16 @@
         <v>161</v>
       </c>
       <c r="W1" t="s">
+        <v>101</v>
+      </c>
+      <c r="X1" t="s">
         <v>3</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -5544,9 +5523,9 @@
       <c r="V2" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="W2" s="2"/>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X2" s="2"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -5568,9 +5547,9 @@
       <c r="V3" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="W3" s="2"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X3" s="2"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>139</v>
       </c>
@@ -5592,9 +5571,9 @@
       <c r="V4" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="W4" s="2"/>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X4" s="2"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>140</v>
       </c>
@@ -5616,9 +5595,9 @@
       <c r="V5" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="W5" s="2"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X5" s="2"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>141</v>
       </c>
@@ -5640,9 +5619,9 @@
       <c r="V6" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="W6" s="2"/>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X6" s="2"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>142</v>
       </c>
@@ -5664,9 +5643,9 @@
       <c r="V7" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="W7" s="2"/>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X7" s="2"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="M8" s="2"/>
       <c r="V8" s="2"/>
     </row>
@@ -5920,10 +5899,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5FE2EA6-5FEC-471F-BC99-9A1BBFAA5478}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5932,15 +5911,16 @@
     <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5954,25 +5934,28 @@
         <v>8</v>
       </c>
       <c r="E1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>65</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>66</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>35</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -5985,10 +5968,10 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>100</v>
       </c>
     </row>
@@ -5999,10 +5982,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA2B7A3-5BF0-4668-9FF0-C3329253032F}">
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6017,15 +6000,16 @@
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6057,25 +6041,28 @@
         <v>68</v>
       </c>
       <c r="K1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L1" t="s">
         <v>3</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>33</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>34</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>35</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>157</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -6086,32 +6073,35 @@
         <v>6</v>
       </c>
       <c r="D2">
-        <f>T2*$S$2</f>
+        <f>U2*$T$2</f>
         <v>35</v>
       </c>
       <c r="E2" t="s">
         <v>45</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" t="s">
+        <v>162</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>100</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>0.20187829087047993</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>1</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>0.5</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -6122,29 +6112,32 @@
         <v>7</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D17" si="0">T3*$S$2</f>
+        <f t="shared" ref="D3:D17" si="0">U3*$T$2</f>
         <v>25</v>
       </c>
       <c r="E3" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" t="s">
+        <v>162</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>100</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>0.13636616953897529</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>4</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>118</v>
       </c>
@@ -6161,23 +6154,26 @@
       <c r="E4" t="s">
         <v>45</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" t="s">
+        <v>162</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>100</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>0.23869667722411225</v>
       </c>
-      <c r="P4" s="6">
+      <c r="Q4" s="6">
         <v>3</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>119</v>
       </c>
@@ -6194,23 +6190,26 @@
       <c r="E5" t="s">
         <v>45</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" t="s">
+        <v>162</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>100</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>8.2072477201456495E-2</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>3</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>120</v>
       </c>
@@ -6227,23 +6226,26 @@
       <c r="E6" t="s">
         <v>45</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" t="s">
+        <v>162</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>100</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>0.42369900879074229</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>3</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>121</v>
       </c>
@@ -6260,23 +6262,26 @@
       <c r="E7" t="s">
         <v>45</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" t="s">
+        <v>162</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>100</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>0.1241405654536567</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>1</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>122</v>
       </c>
@@ -6293,23 +6298,26 @@
       <c r="E8" t="s">
         <v>45</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" t="s">
+        <v>162</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>100</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>0.32595850229310153</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>2</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>123</v>
       </c>
@@ -6326,23 +6334,26 @@
       <c r="E9" t="s">
         <v>45</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K9" t="s">
+        <v>162</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>100</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>0.36936962689871244</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>1</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>124</v>
       </c>
@@ -6359,23 +6370,26 @@
       <c r="E10" t="s">
         <v>45</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" t="s">
+        <v>163</v>
+      </c>
+      <c r="L10" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>100</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>0.80885685592316181</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>1</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>125</v>
       </c>
@@ -6392,23 +6406,26 @@
       <c r="E11" t="s">
         <v>45</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="K11" t="s">
+        <v>163</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>100</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>0.58511935429538409</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>0</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>126</v>
       </c>
@@ -6425,23 +6442,26 @@
       <c r="E12" t="s">
         <v>45</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" t="s">
+        <v>163</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>100</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>0.65065154081854448</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>3</v>
       </c>
-      <c r="T12">
+      <c r="U12">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>127</v>
       </c>
@@ -6458,23 +6478,26 @@
       <c r="E13" t="s">
         <v>45</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="K13" t="s">
+        <v>163</v>
+      </c>
+      <c r="L13" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>100</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>0.95245071881845067</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>3</v>
       </c>
-      <c r="T13">
+      <c r="U13">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>128</v>
       </c>
@@ -6491,23 +6514,26 @@
       <c r="E14" t="s">
         <v>45</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K14" t="s">
+        <v>163</v>
+      </c>
+      <c r="L14" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <v>100</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>0.59844755349762468</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <v>4</v>
       </c>
-      <c r="T14">
+      <c r="U14">
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>129</v>
       </c>
@@ -6524,23 +6550,26 @@
       <c r="E15" t="s">
         <v>45</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="K15" t="s">
+        <v>164</v>
+      </c>
+      <c r="L15" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <v>100</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <v>0.11970343905775549</v>
       </c>
-      <c r="P15">
+      <c r="Q15">
         <v>1</v>
       </c>
-      <c r="T15">
+      <c r="U15">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>130</v>
       </c>
@@ -6557,23 +6586,26 @@
       <c r="E16" t="s">
         <v>45</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="K16" t="s">
+        <v>164</v>
+      </c>
+      <c r="L16" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <v>100</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>0.75180522348958378</v>
       </c>
-      <c r="P16">
+      <c r="Q16">
         <v>0</v>
       </c>
-      <c r="T16">
+      <c r="U16">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>131</v>
       </c>
@@ -6590,19 +6622,22 @@
       <c r="E17" t="s">
         <v>45</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="K17" t="s">
+        <v>164</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="N17">
+      <c r="O17">
         <v>100</v>
       </c>
-      <c r="O17">
+      <c r="P17">
         <v>0.40204258164879814</v>
       </c>
-      <c r="P17">
+      <c r="Q17">
         <v>2</v>
       </c>
-      <c r="T17">
+      <c r="U17">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improved Hazard plotting method
</commit_message>
<xml_diff>
--- a/jupyter_notebooks/file/input/basic_example/network.xlsx
+++ b/jupyter_notebooks/file/input/basic_example/network.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\ResiliencyTool\jupyter_notebooks\file\input\basic_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904ED986-C428-4E49-9DA6-32237F7B741F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E89F659C-A23B-41F2-A0FD-F5581026559D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{9ECEC293-7360-4DDE-9C10-8A2C51BA16DF}"/>
   </bookViews>
@@ -5985,7 +5985,7 @@
   <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
probFailure is now updating for all powerElement objects
</commit_message>
<xml_diff>
--- a/jupyter_notebooks/file/input/basic_example/network.xlsx
+++ b/jupyter_notebooks/file/input/basic_example/network.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\ResiliencyTool\jupyter_notebooks\file\input\basic_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084D43CA-F835-4FFB-BEFE-CD93583C0513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6199C9-A2D0-4771-908C-420C000C8F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1215" windowWidth="27000" windowHeight="14235" activeTab="8" xr2:uid="{9ECEC293-7360-4DDE-9C10-8A2C51BA16DF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{9ECEC293-7360-4DDE-9C10-8A2C51BA16DF}"/>
   </bookViews>
   <sheets>
     <sheet name="simulation" sheetId="12" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="168">
   <si>
     <t>name</t>
   </si>
@@ -542,6 +542,15 @@
   </si>
   <si>
     <t>tower_type3</t>
+  </si>
+  <si>
+    <t>lineSpan</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>dummy</t>
   </si>
 </sst>
 </file>
@@ -551,7 +560,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd\ h:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -573,13 +582,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -591,10 +612,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -604,8 +626,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4633,10 +4657,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4645,13 +4669,12 @@
     <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.7109375" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4680,25 +4703,22 @@
         <v>3</v>
       </c>
       <c r="J1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="L1" t="s">
-        <v>103</v>
-      </c>
-      <c r="M1" t="s">
         <v>104</v>
       </c>
+      <c r="N1" t="s">
+        <v>143</v>
+      </c>
       <c r="O1" t="s">
-        <v>143</v>
-      </c>
-      <c r="P1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -4720,14 +4740,14 @@
       <c r="I2" s="2" t="s">
         <v>105</v>
       </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
       <c r="O2">
         <v>1</v>
       </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -4750,7 +4770,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -4773,7 +4793,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -4796,7 +4816,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>106</v>
       </c>
@@ -4819,7 +4839,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>107</v>
       </c>
@@ -4842,7 +4862,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>108</v>
       </c>
@@ -4865,7 +4885,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>109</v>
       </c>
@@ -4888,7 +4908,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>110</v>
       </c>
@@ -4911,7 +4931,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>111</v>
       </c>
@@ -4934,7 +4954,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>112</v>
       </c>
@@ -4957,7 +4977,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>113</v>
       </c>
@@ -4980,7 +5000,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>114</v>
       </c>
@@ -5003,7 +5023,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>115</v>
       </c>
@@ -5026,7 +5046,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>116</v>
       </c>
@@ -5127,10 +5147,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C68F50D-BD38-47D8-9610-A2EF7C397A58}">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5150,9 +5170,10 @@
     <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5198,8 +5219,11 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -5221,8 +5245,11 @@
       <c r="O2" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -5244,8 +5271,11 @@
       <c r="O3" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -5267,8 +5297,11 @@
       <c r="O4" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>134</v>
       </c>
@@ -5290,8 +5323,11 @@
       <c r="O5" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>135</v>
       </c>
@@ -5313,8 +5349,11 @@
       <c r="O6" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>136</v>
       </c>
@@ -5336,8 +5375,11 @@
       <c r="O7" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>137</v>
       </c>
@@ -5359,8 +5401,11 @@
       <c r="O8" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>138</v>
       </c>
@@ -5381,6 +5426,9 @@
       </c>
       <c r="O9" s="2" t="s">
         <v>105</v>
+      </c>
+      <c r="P9" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -5393,7 +5441,7 @@
   <dimension ref="A1:Y8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5523,6 +5571,9 @@
       <c r="V2" s="2" t="s">
         <v>105</v>
       </c>
+      <c r="W2" t="s">
+        <v>167</v>
+      </c>
       <c r="X2" s="2"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -5547,6 +5598,9 @@
       <c r="V3" s="2" t="s">
         <v>105</v>
       </c>
+      <c r="W3" t="s">
+        <v>167</v>
+      </c>
       <c r="X3" s="2"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -5571,6 +5625,9 @@
       <c r="V4" s="2" t="s">
         <v>105</v>
       </c>
+      <c r="W4" t="s">
+        <v>167</v>
+      </c>
       <c r="X4" s="2"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -5595,6 +5652,9 @@
       <c r="V5" s="2" t="s">
         <v>105</v>
       </c>
+      <c r="W5" t="s">
+        <v>167</v>
+      </c>
       <c r="X5" s="2"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
@@ -5619,6 +5679,9 @@
       <c r="V6" s="2" t="s">
         <v>105</v>
       </c>
+      <c r="W6" t="s">
+        <v>167</v>
+      </c>
       <c r="X6" s="2"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
@@ -5642,6 +5705,9 @@
       </c>
       <c r="V7" s="2" t="s">
         <v>105</v>
+      </c>
+      <c r="W7" t="s">
+        <v>167</v>
       </c>
       <c r="X7" s="2"/>
     </row>
@@ -5658,8 +5724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06392EB3-C4FB-4DF3-BD7E-3D0934814FDF}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5902,7 +5968,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5968,6 +6034,9 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
+      <c r="E2" t="s">
+        <v>167</v>
+      </c>
       <c r="F2" s="2" t="s">
         <v>105</v>
       </c>
@@ -5984,8 +6053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA2B7A3-5BF0-4668-9FF0-C3329253032F}">
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6002,7 +6071,7 @@
     <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.28515625" customWidth="1"/>
     <col min="14" max="14" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
@@ -6061,6 +6130,9 @@
       <c r="Q1" t="s">
         <v>158</v>
       </c>
+      <c r="R1" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -6094,6 +6166,9 @@
       <c r="Q2">
         <v>1</v>
       </c>
+      <c r="R2" t="s">
+        <v>166</v>
+      </c>
       <c r="T2">
         <v>0.5</v>
       </c>
@@ -6133,6 +6208,9 @@
       <c r="Q3">
         <v>4</v>
       </c>
+      <c r="R3" t="s">
+        <v>166</v>
+      </c>
       <c r="U3">
         <v>50</v>
       </c>
@@ -6169,6 +6247,9 @@
       <c r="Q4" s="6">
         <v>3</v>
       </c>
+      <c r="R4" t="s">
+        <v>166</v>
+      </c>
       <c r="U4">
         <v>41</v>
       </c>
@@ -6205,6 +6286,9 @@
       <c r="Q5">
         <v>3</v>
       </c>
+      <c r="R5" t="s">
+        <v>166</v>
+      </c>
       <c r="U5">
         <v>42</v>
       </c>
@@ -6241,6 +6325,9 @@
       <c r="Q6">
         <v>3</v>
       </c>
+      <c r="R6" t="s">
+        <v>166</v>
+      </c>
       <c r="U6">
         <v>43</v>
       </c>
@@ -6277,6 +6364,9 @@
       <c r="Q7">
         <v>1</v>
       </c>
+      <c r="R7" t="s">
+        <v>166</v>
+      </c>
       <c r="U7">
         <v>44</v>
       </c>
@@ -6313,6 +6403,9 @@
       <c r="Q8">
         <v>2</v>
       </c>
+      <c r="R8" t="s">
+        <v>166</v>
+      </c>
       <c r="U8">
         <v>45</v>
       </c>
@@ -6349,6 +6442,9 @@
       <c r="Q9">
         <v>1</v>
       </c>
+      <c r="R9" t="s">
+        <v>166</v>
+      </c>
       <c r="U9">
         <v>46</v>
       </c>
@@ -6376,6 +6472,7 @@
       <c r="L10" s="2" t="s">
         <v>105</v>
       </c>
+      <c r="N10" s="7"/>
       <c r="O10">
         <v>100</v>
       </c>
@@ -6384,6 +6481,9 @@
       </c>
       <c r="Q10">
         <v>1</v>
+      </c>
+      <c r="R10" t="s">
+        <v>166</v>
       </c>
       <c r="U10">
         <v>47</v>
@@ -6421,6 +6521,9 @@
       <c r="Q11">
         <v>0</v>
       </c>
+      <c r="R11" t="s">
+        <v>166</v>
+      </c>
       <c r="U11">
         <v>48</v>
       </c>
@@ -6457,6 +6560,9 @@
       <c r="Q12">
         <v>3</v>
       </c>
+      <c r="R12" t="s">
+        <v>166</v>
+      </c>
       <c r="U12">
         <v>49</v>
       </c>
@@ -6493,6 +6599,9 @@
       <c r="Q13">
         <v>3</v>
       </c>
+      <c r="R13" t="s">
+        <v>166</v>
+      </c>
       <c r="U13">
         <v>50</v>
       </c>
@@ -6529,6 +6638,9 @@
       <c r="Q14">
         <v>4</v>
       </c>
+      <c r="R14" t="s">
+        <v>166</v>
+      </c>
       <c r="U14">
         <v>51</v>
       </c>
@@ -6565,6 +6677,9 @@
       <c r="Q15">
         <v>1</v>
       </c>
+      <c r="R15" t="s">
+        <v>166</v>
+      </c>
       <c r="U15">
         <v>52</v>
       </c>
@@ -6601,6 +6716,9 @@
       <c r="Q16">
         <v>0</v>
       </c>
+      <c r="R16" t="s">
+        <v>166</v>
+      </c>
       <c r="U16">
         <v>53</v>
       </c>
@@ -6636,6 +6754,9 @@
       </c>
       <c r="Q17">
         <v>2</v>
+      </c>
+      <c r="R17" t="s">
+        <v>166</v>
       </c>
       <c r="U17">
         <v>54</v>

</xml_diff>

<commit_message>
Updating older examples and templates v1
</commit_message>
<xml_diff>
--- a/jupyter_notebooks/file/input/basic_example/network.xlsx
+++ b/jupyter_notebooks/file/input/basic_example/network.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\ResiliencyTool\jupyter_notebooks\file\input\basic_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03A4C7E-E257-47AF-8EC6-E0C29B3FE7AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DAA60F8-8765-4132-84AC-C5B3C1C73C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25905" yWindow="3645" windowWidth="21600" windowHeight="11325" xr2:uid="{9ECEC293-7360-4DDE-9C10-8A2C51BA16DF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="13" xr2:uid="{9ECEC293-7360-4DDE-9C10-8A2C51BA16DF}"/>
   </bookViews>
   <sheets>
     <sheet name="simulation" sheetId="12" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="172">
   <si>
     <t>name</t>
   </si>
@@ -546,6 +546,24 @@
   </si>
   <si>
     <t>towers_2</t>
+  </si>
+  <si>
+    <t>element</t>
+  </si>
+  <si>
+    <t>et</t>
+  </si>
+  <si>
+    <t>in_ka</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
+    <t>associated elements</t>
+  </si>
+  <si>
+    <t>ignore montecarlo</t>
   </si>
 </sst>
 </file>
@@ -905,7 +923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC7CE9D1-E831-4D14-93C0-93FEACE3FE30}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -4618,14 +4636,44 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65ABF5EE-300B-4718-811F-36ACB5D73AB1}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G1" t="s">
+        <v>169</v>
+      </c>
+      <c r="H1" t="s">
+        <v>170</v>
+      </c>
+      <c r="I1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added static_generator to all excel sheets
</commit_message>
<xml_diff>
--- a/jupyter_notebooks/file/input/basic_example/network.xlsx
+++ b/jupyter_notebooks/file/input/basic_example/network.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\ResiliencyTool\jupyter_notebooks\file\input\basic_example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engie-my.sharepoint.com/personal/mn6461_engie_com/Documents/Dokumente/GitHub/reXplan-repo/jupyter_notebooks/file/input/basic_example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DAA60F8-8765-4132-84AC-C5B3C1C73C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{6DAA60F8-8765-4132-84AC-C5B3C1C73C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E5F2E1D-36B0-42E2-A9E0-2D81451D2FB3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="13" xr2:uid="{9ECEC293-7360-4DDE-9C10-8A2C51BA16DF}"/>
+    <workbookView xWindow="-25320" yWindow="-8805" windowWidth="25440" windowHeight="15270" firstSheet="5" activeTab="14" xr2:uid="{9ECEC293-7360-4DDE-9C10-8A2C51BA16DF}"/>
   </bookViews>
   <sheets>
     <sheet name="simulation" sheetId="12" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <sheet name="profiles" sheetId="11" r:id="rId12"/>
     <sheet name="crews" sheetId="13" r:id="rId13"/>
     <sheet name="switches" sheetId="14" r:id="rId14"/>
+    <sheet name="static_generators" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -642,8 +643,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Gut" xfId="1" builtinId="26"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -927,7 +928,7 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
@@ -1008,7 +1009,7 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.44140625" customWidth="1"/>
     <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
@@ -1090,7 +1091,7 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
@@ -1352,7 +1353,7 @@
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="9" width="12" customWidth="1"/>
@@ -4603,7 +4604,7 @@
       <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -4638,11 +4639,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65ABF5EE-300B-4718-811F-36ACB5D73AB1}">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -4675,6 +4676,18 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F6E860E-A444-4333-AD50-DFC3F6E0F19D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -4686,7 +4699,7 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -4720,7 +4733,7 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
@@ -5210,7 +5223,7 @@
       <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.109375" bestFit="1" customWidth="1"/>
@@ -5480,7 +5493,7 @@
       <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.109375" bestFit="1" customWidth="1"/>
@@ -5749,7 +5762,7 @@
       <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
@@ -5859,7 +5872,7 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
@@ -5992,7 +6005,7 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
@@ -6081,7 +6094,7 @@
       <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>

</xml_diff>